<commit_message>
numeros de 24 sitios
</commit_message>
<xml_diff>
--- a/Sitios/listaContactos.xlsx
+++ b/Sitios/listaContactos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7711276559</t>
+          <t>7712298632</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -471,7 +471,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7713976304</t>
+          <t>7711258720</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -489,7 +489,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7712341335</t>
+          <t>7717155410</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>7712066354</t>
+          <t>5583699920</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -526,7 +526,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>7711927247</t>
+          <t>7715690454</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>7711181766</t>
+          <t>7711615285</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -562,7 +562,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7711001034</t>
+          <t>7711575091</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>7717471797</t>
+          <t>7713187830</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -598,7 +598,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7712667033</t>
+          <t>7717120945</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -617,7 +617,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>7711604307</t>
+          <t>7711248373</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -635,7 +635,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>7711987953</t>
+          <t>7711519561</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -653,7 +653,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>7712214288</t>
+          <t>7711468170</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -671,7 +671,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>7711072794</t>
+          <t>7711015664</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -689,7 +689,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5539181341</t>
+          <t>7711227813</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -707,7 +707,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>7711854204</t>
+          <t>7717091232</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -725,7 +725,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>7711313225</t>
+          <t>7713031132</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -743,7 +743,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>7713021136</t>
+          <t>7713496839</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -762,7 +762,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>7711301465</t>
+          <t>7711301339</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -780,7 +780,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>7712434024</t>
+          <t>7711004270</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -799,7 +799,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>7712058567</t>
+          <t>7717021603</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -818,7 +818,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>7716992349</t>
+          <t>7711405885</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -836,7 +836,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>7711328389</t>
+          <t>7715268539</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>7711277803</t>
+          <t>7712076789</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -873,7 +873,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>7711111329</t>
+          <t>7712894116</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>7711396465</t>
+          <t>7711869908</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -905,6 +905,466 @@
       <c r="C26" t="inlineStr">
         <is>
           <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>7711809278</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>7712141045</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>7712950081</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>7712444491</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>7712994514</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>7712292105</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>7711393462</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>7711372699</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>7717470972</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>7712285031</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>7717724295</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>7712955716</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>7712167964</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>7716992902</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>7711566394</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>7714100900</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>7712052619</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>7712078109</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>7711991969</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>7711393226</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>7721015566</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>7711255859</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>¡Hola! 👋🏼 ¿Estás listo para llevar tu negocio al siguiente nivel? 🌐✨ 🚀 
+Transforma tu presencia en línea y atrapa a esos clientes que están buscando lo que ofreces. ¡Imagina un sitio web profesional y atractivo que convierta visitantes en compradores fieles! 🛍️🔥 
+¿Listo para comenzar? Responde a este mensaje y uno de nuestros expertos te guiará en el proceso. ¡Es tu momento de brillar en internet! 🌐🌟</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\B.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>7712180247</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>7712954824</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>7716834318</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>⏳ No pierdas más clientes. Contáctanos ahora y asegura tu lugar. ¡Es tu momento de destacar en internet! 🌟 📩 
+Escríbenos ya para obtener esta oferta exclusiva. ¡No esperes más! 😊</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>C:\Users\4to CREATIVO\Desktop\WhatsAutoA\Images\A.jpeg</t>
         </is>
       </c>
     </row>

</xml_diff>